<commit_message>
format 1 bugs fixed
</commit_message>
<xml_diff>
--- a/xlsx_files/BCA_2-2024_shift1.xlsx
+++ b/xlsx_files/BCA_2-2024_shift1.xlsx
@@ -527,7 +527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI130"/>
+  <dimension ref="A1:AI121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,7 +628,7 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>Class-: BCA  II Semester Batch [2021 - 2024] Jan- June 2023</t>
+          <t>Class-: BCA  2 Semester Batch [2021 - 2024]</t>
         </is>
       </c>
       <c r="B3" s="4" t="n"/>
@@ -8845,7 +8845,7 @@
       </c>
       <c r="AH55" s="10" t="inlineStr">
         <is>
-          <t>106,102</t>
+          <t>102,106</t>
         </is>
       </c>
       <c r="AI55" s="10" t="n"/>
@@ -15545,7 +15545,7 @@
       </c>
       <c r="AI96" s="10" t="inlineStr">
         <is>
-          <t>172,102</t>
+          <t>102,172</t>
         </is>
       </c>
     </row>
@@ -15711,12 +15711,12 @@
       </c>
       <c r="AH97" s="10" t="inlineStr">
         <is>
-          <t>108,106,102</t>
+          <t>102,106,108</t>
         </is>
       </c>
       <c r="AI97" s="10" t="inlineStr">
         <is>
-          <t>104,110</t>
+          <t>110,104</t>
         </is>
       </c>
     </row>
@@ -19156,66 +19156,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>102-Applied Maths Dr. Anchal Tehlan (Sec A &amp; B)</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>104-WBP - Mr. Sundeep Kumar(A) &amp; Ms. Kanika Kundu (B)</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>106-Data Struc Using C - Dr.Neetu Anand(A )   Mr.Manoj Kumar (B )</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>108-DBMS - Ms.Kanika Kundu (A) &amp; Ms.Vinita Tomar(B)</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>110-EVS - Dr.Manju Dhillon (Sec A &amp; Sec B)</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>172-WBP Lab - Mr.Sundeep Kumar/ Dr.Neetu Narwal (Sec A) &amp;  Ms.Kanika Kundu(Sec A) &amp; Dr.Neetu Narwal (Sec B)</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>174- DS Lab - Dr.Neetu Anand /Dr.Kumar Gaurav (A ) &amp;  Mr.Manoj Kumar (B )</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>176- DBMS Lab - Ms.Kanika Kundu / Mr. Siddharth Shankar (A)   &amp;  Ms.Vinita Tomar (B)</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr"/>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>Class Coordinator: Ms.Anchal Tehlan (Sec A) - Mr.Manoj Kumar (Sec B)</t>
+          <t>0 0 pooja singh</t>
         </is>
       </c>
     </row>

</xml_diff>